<commit_message>
build bdd with config files
</commit_message>
<xml_diff>
--- a/bdd/bdd_train_unif_filtres.xlsx
+++ b/bdd/bdd_train_unif_filtres.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elevate\Documents\PowerBI_LLM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elevate\Documents\PowerBI_LLM\PowerBI-LLM\bdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC60CD1A-5A87-44D7-A9FA-D9BE7BDF294A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D05B6C-E722-4BE1-A7F3-AB27AC506131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BEC43D25-63C5-48CA-857E-16019B125449}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>json_path_before_change</t>
   </si>
@@ -110,31 +110,10 @@
     <t>Mets le filtre browser au même format que le filtre region</t>
   </si>
   <si>
-    <t>jsons_train/IT__web_sections.json</t>
-  </si>
-  <si>
-    <t>jsons_train/IT__web_same_as_country_section1.json</t>
-  </si>
-  <si>
-    <t>jsons_train/IT__web_same_as_region_section1.json</t>
-  </si>
-  <si>
-    <t>jsons_train/IT__web_same_as_region_section2.json</t>
-  </si>
-  <si>
-    <t>jsons_train/IT__web_same_as_browser_section2.json</t>
-  </si>
-  <si>
-    <t>Uniformise le format de tous les filtres de la section 1 en te basant sur le format du filtre Country de la section 1</t>
-  </si>
-  <si>
-    <t>Uniformise le format de tous les filtres de la section 1 en te basant sur le format du filtre Region de la section 1</t>
-  </si>
-  <si>
-    <t>Uniformise le format de tous les filtres de la section 2 en te basant sur le format du filtre Region de la section 2</t>
-  </si>
-  <si>
-    <t>Uniformise le format de tous les filtres de la section 2 en te basant sur le format du filtre Browser de la section 2</t>
+    <t>filtre_visuels</t>
+  </si>
+  <si>
+    <t>slicer, advancedSlicerVisual</t>
   </si>
 </sst>
 </file>
@@ -521,20 +500,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7405241D-8C65-43C0-B6BC-A90E331BB2DA}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41.1796875" customWidth="1"/>
-    <col min="2" max="2" width="48.453125" customWidth="1"/>
-    <col min="3" max="3" width="82.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="48.453125" customWidth="1"/>
+    <col min="4" max="4" width="82.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,10 +521,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -553,10 +535,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -564,10 +549,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -575,10 +563,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -586,10 +577,13 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -597,10 +591,13 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -608,10 +605,13 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -619,10 +619,13 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -630,10 +633,13 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -641,10 +647,13 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -652,51 +661,10 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean code + fonctions fichiers config
</commit_message>
<xml_diff>
--- a/bdd/bdd_train_unif_filtres.xlsx
+++ b/bdd/bdd_train_unif_filtres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elevate\Documents\PowerBI_LLM\PowerBI-LLM\bdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D05B6C-E722-4BE1-A7F3-AB27AC506131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83356353-E952-454D-A4E5-E21EEA1E217D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BEC43D25-63C5-48CA-857E-16019B125449}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BEC43D25-63C5-48CA-857E-16019B125449}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -47,39 +47,15 @@
     <t>instructions</t>
   </si>
   <si>
-    <t>jsons_train/IT__web.json</t>
-  </si>
-  <si>
-    <t>jsons_train/airbnb.json</t>
-  </si>
-  <si>
-    <t>jsons_train/IT__web_same_as_browser.json</t>
-  </si>
-  <si>
     <t>Uniformise le format de tous les filtres en te basant sur le format du filtre Browser</t>
   </si>
   <si>
-    <t>jsons_train/IT__web_same_as_category.json</t>
-  </si>
-  <si>
     <t>Uniformise le format de tous les filtres en te basant sur le format du filtre Category</t>
   </si>
   <si>
-    <t>jsons_train/IT__web_same_as_region.json</t>
-  </si>
-  <si>
     <t>Uniformise le format de tous les filtres en te basant sur le format du filtre Region</t>
   </si>
   <si>
-    <t>jsons_train/airbnb_same_as_cancellation.json</t>
-  </si>
-  <si>
-    <t>jsons_train/airbnb_same_as_quartier.json</t>
-  </si>
-  <si>
-    <t>jsons_train/airbnb_same_as_room_type.json</t>
-  </si>
-  <si>
     <t>Uniformise le format de tous les filtres en te basant sur le format du filtre Cancellation</t>
   </si>
   <si>
@@ -89,24 +65,9 @@
     <t>Uniformise le format de tous les filtres en te basant sur le format du filtre room type</t>
   </si>
   <si>
-    <t>jsons_train/IT__web_bis.json</t>
-  </si>
-  <si>
     <t>Uniformise le format de tous les filtres en te basant sur le format du filtre Country</t>
   </si>
   <si>
-    <t>jsons_train/IT__web_bis_same_as_country.json</t>
-  </si>
-  <si>
-    <t>jsons_train/IT__web_bis_same_as_region.json</t>
-  </si>
-  <si>
-    <t>jsons_train/IT__web_bis_same_as_browser.json</t>
-  </si>
-  <si>
-    <t>jsons_train/IT__web_bis_browser_same_as_region.json</t>
-  </si>
-  <si>
     <t>Mets le filtre browser au même format que le filtre region</t>
   </si>
   <si>
@@ -114,6 +75,45 @@
   </si>
   <si>
     <t>slicer, advancedSlicerVisual</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/IT__web.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/IT__web_same_as_browser.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/IT__web_same_as_category.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/IT__web_same_as_region.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/IT__web_bis.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/IT__web_bis_same_as_country.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/IT__web_bis_same_as_region.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/IT__web_bis_same_as_browser.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/IT__web_bis_browser_same_as_region.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/airbnb.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/airbnb_same_as_cancellation.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/airbnb_same_as_quartier.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/airbnb_same_as_room_type.json</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,7 +521,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -529,44 +529,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -574,13 +574,13 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -588,13 +588,13 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -602,13 +602,13 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -616,55 +616,55 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fonction pour réintégrer parties modifiées dans json
</commit_message>
<xml_diff>
--- a/bdd/bdd_train_unif_filtres.xlsx
+++ b/bdd/bdd_train_unif_filtres.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elevate\Documents\PowerBI_LLM\PowerBI-LLM\bdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83356353-E952-454D-A4E5-E21EEA1E217D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B4DD61-DBDB-45A7-A06D-C60AAF5ECB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BEC43D25-63C5-48CA-857E-16019B125449}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10080" xr2:uid="{BEC43D25-63C5-48CA-857E-16019B125449}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>json_path_before_change</t>
   </si>
@@ -71,10 +71,13 @@
     <t>Mets le filtre browser au même format que le filtre region</t>
   </si>
   <si>
-    <t>filtre_visuels</t>
-  </si>
-  <si>
-    <t>slicer, advancedSlicerVisual</t>
+    <t>Uniformise le format de tous les filtres en te basant sur le format du filtre content rating</t>
+  </si>
+  <si>
+    <t>Uniformise le format de tous les filtres en te basant sur le format du filtre type</t>
+  </si>
+  <si>
+    <t>Uniformise le format de tous les filtres en te basant sur le format du filtre genres</t>
   </si>
   <si>
     <t>jsons_train/unif_filtres/IT__web.json</t>
@@ -114,6 +117,18 @@
   </si>
   <si>
     <t>jsons_train/unif_filtres/airbnb_same_as_room_type.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/apps.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/apps_same_as_content_rating.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/apps_same_as_genre.json</t>
+  </si>
+  <si>
+    <t>jsons_train/unif_filtres/apps_same_as_type.json</t>
   </si>
 </sst>
 </file>
@@ -163,9 +178,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,20 +516,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7405241D-8C65-43C0-B6BC-A90E331BB2DA}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41.1796875" customWidth="1"/>
-    <col min="2" max="3" width="48.453125" customWidth="1"/>
-    <col min="4" max="4" width="82.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.453125" customWidth="1"/>
+    <col min="3" max="3" width="95.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,150 +537,150 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>